<commit_message>
Fix columns with missing data, begin transfering over code
</commit_message>
<xml_diff>
--- a/data/df_analysis.xlsx
+++ b/data/df_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eboumasi\Documents\GitHub\The-Kids-Are-All-Right\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C03F49-B494-4C13-BBA7-B9F25B336FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA8AD3C-24D5-4707-B47C-CEE62A3A94AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13146" uniqueCount="3908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13311" uniqueCount="3909">
   <si>
     <t>pid</t>
   </si>
@@ -11808,12 +11808,15 @@
   <si>
     <t>duration</t>
   </si>
+  <si>
+    <t>None</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11831,6 +11834,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -11868,13 +11879,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12180,13 +12194,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BN4" sqref="BN4"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BH1" sqref="BH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="49" max="49" width="13.6328125" customWidth="1"/>
+    <col min="50" max="50" width="12.54296875" customWidth="1"/>
+    <col min="51" max="51" width="14.81640625" customWidth="1"/>
+    <col min="52" max="52" width="13.6328125" customWidth="1"/>
+    <col min="53" max="53" width="14.453125" customWidth="1"/>
+    <col min="54" max="54" width="14" customWidth="1"/>
+    <col min="55" max="55" width="17.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12265,19 +12288,19 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
@@ -12331,25 +12354,25 @@
       <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
@@ -12404,7 +12427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>69</v>
       </c>
@@ -12474,6 +12497,12 @@
       <c r="Z2" t="s">
         <v>91</v>
       </c>
+      <c r="AA2" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC2" t="s">
         <v>91</v>
       </c>
@@ -12574,7 +12603,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>257</v>
       </c>
@@ -12750,7 +12779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>42</v>
       </c>
@@ -12926,7 +12955,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>74</v>
       </c>
@@ -13102,7 +13131,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>136</v>
       </c>
@@ -13175,6 +13204,9 @@
       <c r="AA6" t="s">
         <v>92</v>
       </c>
+      <c r="AB6" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC6" t="s">
         <v>92</v>
       </c>
@@ -13272,7 +13304,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>139</v>
       </c>
@@ -13448,7 +13480,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>213</v>
       </c>
@@ -13624,7 +13656,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>92</v>
       </c>
@@ -13800,7 +13832,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>59</v>
       </c>
@@ -13976,7 +14008,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11</v>
       </c>
@@ -14152,7 +14184,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>135</v>
       </c>
@@ -14222,6 +14254,12 @@
       <c r="Z12" t="s">
         <v>129</v>
       </c>
+      <c r="AA12" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC12" t="s">
         <v>129</v>
       </c>
@@ -14322,7 +14360,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>45</v>
       </c>
@@ -14392,6 +14430,12 @@
       <c r="Z13" t="s">
         <v>129</v>
       </c>
+      <c r="AA13" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC13" t="s">
         <v>91</v>
       </c>
@@ -14492,7 +14536,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>234</v>
       </c>
@@ -14559,6 +14603,12 @@
       <c r="Z14" t="s">
         <v>91</v>
       </c>
+      <c r="AA14" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC14" t="s">
         <v>129</v>
       </c>
@@ -14647,7 +14697,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>194</v>
       </c>
@@ -14823,7 +14873,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>46</v>
       </c>
@@ -14999,7 +15049,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>86</v>
       </c>
@@ -15072,6 +15122,9 @@
       <c r="AA17" t="s">
         <v>129</v>
       </c>
+      <c r="AB17" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC17" t="s">
         <v>92</v>
       </c>
@@ -15172,7 +15225,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>247</v>
       </c>
@@ -15348,7 +15401,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>124</v>
       </c>
@@ -15421,6 +15474,9 @@
       <c r="AA19" t="s">
         <v>92</v>
       </c>
+      <c r="AB19" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC19" t="s">
         <v>91</v>
       </c>
@@ -15518,7 +15574,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>250</v>
       </c>
@@ -15694,7 +15750,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>240</v>
       </c>
@@ -15767,6 +15823,9 @@
       <c r="AA21" t="s">
         <v>92</v>
       </c>
+      <c r="AB21" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC21" t="s">
         <v>92</v>
       </c>
@@ -15867,7 +15926,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>28</v>
       </c>
@@ -16043,7 +16102,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>245</v>
       </c>
@@ -16113,6 +16172,9 @@
       <c r="Z23" t="s">
         <v>156</v>
       </c>
+      <c r="AA23" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB23" t="s">
         <v>371</v>
       </c>
@@ -16216,7 +16278,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>78</v>
       </c>
@@ -16392,7 +16454,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>182</v>
       </c>
@@ -16568,7 +16630,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>140</v>
       </c>
@@ -16641,6 +16703,9 @@
       <c r="AA26" t="s">
         <v>129</v>
       </c>
+      <c r="AB26" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC26" t="s">
         <v>91</v>
       </c>
@@ -16741,7 +16806,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>235</v>
       </c>
@@ -16811,6 +16876,12 @@
       <c r="Z27" t="s">
         <v>390</v>
       </c>
+      <c r="AA27" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC27" t="s">
         <v>156</v>
       </c>
@@ -16911,7 +16982,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>226</v>
       </c>
@@ -16981,6 +17052,12 @@
       <c r="Z28" t="s">
         <v>92</v>
       </c>
+      <c r="AA28" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC28" t="s">
         <v>91</v>
       </c>
@@ -17081,7 +17158,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="29" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>70</v>
       </c>
@@ -17151,6 +17228,12 @@
       <c r="Z29" t="s">
         <v>129</v>
       </c>
+      <c r="AA29" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC29" t="s">
         <v>92</v>
       </c>
@@ -17239,7 +17322,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>19</v>
       </c>
@@ -17312,6 +17395,12 @@
       <c r="AB30" t="s">
         <v>371</v>
       </c>
+      <c r="AC30" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>3908</v>
+      </c>
       <c r="AH30" t="s">
         <v>93</v>
       </c>
@@ -17403,7 +17492,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="31" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>225</v>
       </c>
@@ -17579,7 +17668,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="32" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>172</v>
       </c>
@@ -17755,7 +17844,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>160</v>
       </c>
@@ -17931,7 +18020,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>88</v>
       </c>
@@ -18001,6 +18090,9 @@
       <c r="Z34" t="s">
         <v>390</v>
       </c>
+      <c r="AA34" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB34" t="s">
         <v>91</v>
       </c>
@@ -18104,7 +18196,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>49</v>
       </c>
@@ -18171,6 +18263,9 @@
       <c r="Z35" t="s">
         <v>91</v>
       </c>
+      <c r="AA35" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB35" t="s">
         <v>390</v>
       </c>
@@ -18262,7 +18357,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>100</v>
       </c>
@@ -18438,7 +18533,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>269</v>
       </c>
@@ -18508,6 +18603,12 @@
       <c r="Z37" t="s">
         <v>390</v>
       </c>
+      <c r="AA37" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC37" t="s">
         <v>92</v>
       </c>
@@ -18608,7 +18709,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>232</v>
       </c>
@@ -18784,7 +18885,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>62</v>
       </c>
@@ -18960,7 +19061,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>81</v>
       </c>
@@ -19030,6 +19131,12 @@
       <c r="Z40" t="s">
         <v>92</v>
       </c>
+      <c r="AA40" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC40" t="s">
         <v>91</v>
       </c>
@@ -19130,7 +19237,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>253</v>
       </c>
@@ -19306,7 +19413,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>212</v>
       </c>
@@ -19482,7 +19589,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>131</v>
       </c>
@@ -19646,7 +19753,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>184</v>
       </c>
@@ -19822,7 +19929,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>174</v>
       </c>
@@ -19895,6 +20002,12 @@
       <c r="Z45" t="s">
         <v>91</v>
       </c>
+      <c r="AA45" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC45" t="s">
         <v>91</v>
       </c>
@@ -19995,7 +20108,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>99</v>
       </c>
@@ -20171,7 +20284,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>63</v>
       </c>
@@ -20347,7 +20460,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>165</v>
       </c>
@@ -20520,7 +20633,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>242</v>
       </c>
@@ -20696,7 +20809,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>80</v>
       </c>
@@ -20769,6 +20882,9 @@
       <c r="AA50" t="s">
         <v>129</v>
       </c>
+      <c r="AB50" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC50" t="s">
         <v>91</v>
       </c>
@@ -20869,7 +20985,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>252</v>
       </c>
@@ -21033,7 +21149,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>132</v>
       </c>
@@ -21106,6 +21222,9 @@
       <c r="AA52" t="s">
         <v>92</v>
       </c>
+      <c r="AB52" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC52" t="s">
         <v>390</v>
       </c>
@@ -21206,7 +21325,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>30</v>
       </c>
@@ -21382,7 +21501,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>223</v>
       </c>
@@ -21543,7 +21662,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="55" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>230</v>
       </c>
@@ -21616,6 +21735,9 @@
       <c r="AA55" t="s">
         <v>129</v>
       </c>
+      <c r="AB55" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC55" t="s">
         <v>92</v>
       </c>
@@ -21716,7 +21838,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="56" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>43</v>
       </c>
@@ -21892,7 +22014,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>21</v>
       </c>
@@ -22068,7 +22190,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="58" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>14</v>
       </c>
@@ -22147,6 +22269,9 @@
       <c r="AC58" t="s">
         <v>91</v>
       </c>
+      <c r="AD58" t="s">
+        <v>3908</v>
+      </c>
       <c r="AE58" t="s">
         <v>93</v>
       </c>
@@ -22238,7 +22363,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="59" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>286</v>
       </c>
@@ -22308,6 +22433,9 @@
       <c r="Z59" t="s">
         <v>91</v>
       </c>
+      <c r="AA59" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB59" t="s">
         <v>91</v>
       </c>
@@ -22411,7 +22539,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="60" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>53</v>
       </c>
@@ -22587,7 +22715,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>116</v>
       </c>
@@ -22657,6 +22785,9 @@
       <c r="Z61" t="s">
         <v>371</v>
       </c>
+      <c r="AA61" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB61" t="s">
         <v>371</v>
       </c>
@@ -22760,7 +22891,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="62" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>128</v>
       </c>
@@ -22936,7 +23067,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>48</v>
       </c>
@@ -23115,7 +23246,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="64" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>167</v>
       </c>
@@ -23182,6 +23313,9 @@
       <c r="Z64" t="s">
         <v>92</v>
       </c>
+      <c r="AA64" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB64" t="s">
         <v>129</v>
       </c>
@@ -23285,7 +23419,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="65" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>256</v>
       </c>
@@ -23446,7 +23580,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>119</v>
       </c>
@@ -23622,7 +23756,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>102</v>
       </c>
@@ -23798,7 +23932,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="68" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>22</v>
       </c>
@@ -23974,7 +24108,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>238</v>
       </c>
@@ -24150,7 +24284,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="70" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>204</v>
       </c>
@@ -24326,7 +24460,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>275</v>
       </c>
@@ -24396,6 +24530,12 @@
       <c r="Z71" t="s">
         <v>371</v>
       </c>
+      <c r="AA71" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC71" t="s">
         <v>390</v>
       </c>
@@ -24496,7 +24636,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>206</v>
       </c>
@@ -24654,7 +24794,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>52</v>
       </c>
@@ -24830,7 +24970,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="74" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>103</v>
       </c>
@@ -24991,7 +25131,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="75" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>51</v>
       </c>
@@ -25167,7 +25307,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="76" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -25343,7 +25483,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="77" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>249</v>
       </c>
@@ -25519,7 +25659,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="78" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>87</v>
       </c>
@@ -25592,6 +25732,9 @@
       <c r="AA78" t="s">
         <v>92</v>
       </c>
+      <c r="AB78" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC78" t="s">
         <v>91</v>
       </c>
@@ -25692,7 +25835,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="79" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>190</v>
       </c>
@@ -25762,6 +25905,12 @@
       <c r="Z79" t="s">
         <v>92</v>
       </c>
+      <c r="AA79" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC79" t="s">
         <v>92</v>
       </c>
@@ -25862,7 +26011,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>159</v>
       </c>
@@ -25935,6 +26084,9 @@
       <c r="AA80" t="s">
         <v>129</v>
       </c>
+      <c r="AB80" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC80" t="s">
         <v>92</v>
       </c>
@@ -26035,7 +26187,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="81" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>82</v>
       </c>
@@ -26105,6 +26257,9 @@
       <c r="Z81" t="s">
         <v>91</v>
       </c>
+      <c r="AA81" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB81" t="s">
         <v>92</v>
       </c>
@@ -26208,7 +26363,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="82" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>219</v>
       </c>
@@ -26281,6 +26436,9 @@
       <c r="AA82" t="s">
         <v>92</v>
       </c>
+      <c r="AB82" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC82" t="s">
         <v>92</v>
       </c>
@@ -26381,7 +26539,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="83" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>93</v>
       </c>
@@ -26451,6 +26609,9 @@
       <c r="Z83" t="s">
         <v>390</v>
       </c>
+      <c r="AA83" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB83" t="s">
         <v>91</v>
       </c>
@@ -26554,7 +26715,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="84" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>16</v>
       </c>
@@ -26624,6 +26785,9 @@
       <c r="Z84" t="s">
         <v>371</v>
       </c>
+      <c r="AA84" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB84" t="s">
         <v>156</v>
       </c>
@@ -26727,7 +26891,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="85" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>110</v>
       </c>
@@ -26797,6 +26961,12 @@
       <c r="Z85" t="s">
         <v>371</v>
       </c>
+      <c r="AA85" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC85" t="s">
         <v>371</v>
       </c>
@@ -26897,7 +27067,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="86" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>150</v>
       </c>
@@ -27073,7 +27243,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="87" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>260</v>
       </c>
@@ -27143,6 +27313,12 @@
       <c r="Z87" t="s">
         <v>91</v>
       </c>
+      <c r="AA87" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC87" t="s">
         <v>91</v>
       </c>
@@ -27243,7 +27419,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="88" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>237</v>
       </c>
@@ -27419,7 +27595,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="89" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>203</v>
       </c>
@@ -27595,7 +27771,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="90" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>289</v>
       </c>
@@ -27668,6 +27844,9 @@
       <c r="AA90" t="s">
         <v>91</v>
       </c>
+      <c r="AB90" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC90" t="s">
         <v>390</v>
       </c>
@@ -27768,7 +27947,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>71</v>
       </c>
@@ -27944,7 +28123,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="92" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>288</v>
       </c>
@@ -28017,6 +28196,9 @@
       <c r="AA92" t="s">
         <v>390</v>
       </c>
+      <c r="AB92" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC92" t="s">
         <v>390</v>
       </c>
@@ -28117,7 +28299,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="93" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>284</v>
       </c>
@@ -28293,7 +28475,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>73</v>
       </c>
@@ -28366,6 +28548,9 @@
       <c r="AA94" t="s">
         <v>129</v>
       </c>
+      <c r="AB94" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC94" t="s">
         <v>92</v>
       </c>
@@ -28466,7 +28651,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="95" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>281</v>
       </c>
@@ -28536,6 +28721,9 @@
       <c r="Z95" t="s">
         <v>92</v>
       </c>
+      <c r="AA95" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB95" t="s">
         <v>91</v>
       </c>
@@ -28639,7 +28827,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="96" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>24</v>
       </c>
@@ -28815,7 +29003,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>180</v>
       </c>
@@ -28991,7 +29179,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="98" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>255</v>
       </c>
@@ -29064,6 +29252,9 @@
       <c r="AA98" t="s">
         <v>129</v>
       </c>
+      <c r="AB98" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC98" t="s">
         <v>91</v>
       </c>
@@ -29164,7 +29355,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="99" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>282</v>
       </c>
@@ -29340,7 +29531,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="100" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>4</v>
       </c>
@@ -29404,6 +29595,12 @@
       <c r="Z100" t="s">
         <v>92</v>
       </c>
+      <c r="AA100" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC100" t="s">
         <v>156</v>
       </c>
@@ -29501,7 +29698,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="101" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>209</v>
       </c>
@@ -29677,7 +29874,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="102" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>20</v>
       </c>
@@ -29853,7 +30050,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="103" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>94</v>
       </c>
@@ -29926,6 +30123,9 @@
       <c r="AA103" t="s">
         <v>91</v>
       </c>
+      <c r="AB103" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC103" t="s">
         <v>156</v>
       </c>
@@ -30026,7 +30226,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="104" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>90</v>
       </c>
@@ -30096,6 +30296,12 @@
       <c r="Z104" t="s">
         <v>92</v>
       </c>
+      <c r="AA104" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB104" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC104" t="s">
         <v>92</v>
       </c>
@@ -30196,7 +30402,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="105" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>108</v>
       </c>
@@ -30272,6 +30478,9 @@
       <c r="AA105" t="s">
         <v>91</v>
       </c>
+      <c r="AB105" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC105" t="s">
         <v>92</v>
       </c>
@@ -30372,7 +30581,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="106" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>95</v>
       </c>
@@ -30548,7 +30757,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="107" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>127</v>
       </c>
@@ -30618,6 +30827,9 @@
       <c r="Z107" t="s">
         <v>91</v>
       </c>
+      <c r="AA107" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB107" t="s">
         <v>91</v>
       </c>
@@ -30721,7 +30933,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="108" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>231</v>
       </c>
@@ -30791,6 +31003,9 @@
       <c r="Z108" t="s">
         <v>91</v>
       </c>
+      <c r="AA108" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB108" t="s">
         <v>156</v>
       </c>
@@ -30894,7 +31109,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>56</v>
       </c>
@@ -30964,6 +31179,12 @@
       <c r="Z109" t="s">
         <v>390</v>
       </c>
+      <c r="AA109" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB109" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC109" t="s">
         <v>129</v>
       </c>
@@ -31061,7 +31282,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="110" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>262</v>
       </c>
@@ -31131,6 +31352,9 @@
       <c r="Z110" t="s">
         <v>156</v>
       </c>
+      <c r="AA110" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB110" t="s">
         <v>91</v>
       </c>
@@ -31234,7 +31458,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="111" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>40</v>
       </c>
@@ -31410,7 +31634,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>202</v>
       </c>
@@ -31480,6 +31704,12 @@
       <c r="Z112" t="s">
         <v>371</v>
       </c>
+      <c r="AA112" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB112" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC112" t="s">
         <v>92</v>
       </c>
@@ -31580,7 +31810,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>148</v>
       </c>
@@ -31756,7 +31986,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="114" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>98</v>
       </c>
@@ -31826,6 +32056,12 @@
       <c r="Z114" t="s">
         <v>92</v>
       </c>
+      <c r="AA114" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC114" t="s">
         <v>92</v>
       </c>
@@ -31926,7 +32162,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="115" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>38</v>
       </c>
@@ -32102,7 +32338,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="116" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>199</v>
       </c>
@@ -32172,6 +32408,12 @@
       <c r="Z116" t="s">
         <v>91</v>
       </c>
+      <c r="AA116" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB116" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC116" t="s">
         <v>91</v>
       </c>
@@ -32272,7 +32514,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="117" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>248</v>
       </c>
@@ -32342,6 +32584,9 @@
       <c r="Z117" t="s">
         <v>156</v>
       </c>
+      <c r="AA117" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB117" t="s">
         <v>91</v>
       </c>
@@ -32445,7 +32690,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="118" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>149</v>
       </c>
@@ -32621,7 +32866,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="119" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>58</v>
       </c>
@@ -32797,7 +33042,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="120" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>144</v>
       </c>
@@ -32973,7 +33218,7 @@
         <v>1843</v>
       </c>
     </row>
-    <row r="121" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>105</v>
       </c>
@@ -33149,7 +33394,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>259</v>
       </c>
@@ -33319,7 +33564,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="123" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>169</v>
       </c>
@@ -33392,9 +33637,15 @@
       <c r="AA123" t="s">
         <v>91</v>
       </c>
+      <c r="AB123" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC123" t="s">
         <v>91</v>
       </c>
+      <c r="AD123" t="s">
+        <v>3908</v>
+      </c>
       <c r="AH123" t="s">
         <v>99</v>
       </c>
@@ -33489,7 +33740,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>215</v>
       </c>
@@ -33665,7 +33916,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="125" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>39</v>
       </c>
@@ -33841,7 +34092,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="126" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>157</v>
       </c>
@@ -34017,7 +34268,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="127" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>133</v>
       </c>
@@ -34193,7 +34444,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="128" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>193</v>
       </c>
@@ -34369,7 +34620,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>158</v>
       </c>
@@ -34545,7 +34796,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="130" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>109</v>
       </c>
@@ -34618,6 +34869,9 @@
       <c r="AA130" t="s">
         <v>91</v>
       </c>
+      <c r="AB130" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC130" t="s">
         <v>371</v>
       </c>
@@ -34718,7 +34972,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="131" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>125</v>
       </c>
@@ -34788,6 +35042,9 @@
       <c r="Z131" t="s">
         <v>156</v>
       </c>
+      <c r="AA131" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB131" t="s">
         <v>156</v>
       </c>
@@ -34891,7 +35148,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="132" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>101</v>
       </c>
@@ -35067,7 +35324,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="133" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>17</v>
       </c>
@@ -35137,9 +35394,15 @@
       <c r="Z133" t="s">
         <v>371</v>
       </c>
+      <c r="AA133" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB133" t="s">
         <v>129</v>
       </c>
+      <c r="AC133" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD133" t="s">
         <v>129</v>
       </c>
@@ -35237,7 +35500,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="134" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>130</v>
       </c>
@@ -35307,6 +35570,9 @@
       <c r="Z134" t="s">
         <v>92</v>
       </c>
+      <c r="AA134" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB134" t="s">
         <v>92</v>
       </c>
@@ -35410,7 +35676,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="135" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>65</v>
       </c>
@@ -35586,7 +35852,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="136" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>265</v>
       </c>
@@ -35659,6 +35925,9 @@
       <c r="AA136" t="s">
         <v>129</v>
       </c>
+      <c r="AB136" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC136" t="s">
         <v>371</v>
       </c>
@@ -35759,7 +36028,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="137" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>118</v>
       </c>
@@ -35935,7 +36204,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="138" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>176</v>
       </c>
@@ -35993,6 +36262,12 @@
       <c r="Z138" t="s">
         <v>371</v>
       </c>
+      <c r="AA138" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB138" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC138" t="s">
         <v>371</v>
       </c>
@@ -36093,7 +36368,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="139" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>283</v>
       </c>
@@ -36269,7 +36544,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="140" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>8</v>
       </c>
@@ -36445,7 +36720,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="141" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>254</v>
       </c>
@@ -36606,7 +36881,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="142" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>23</v>
       </c>
@@ -36676,6 +36951,9 @@
       <c r="Z142" t="s">
         <v>156</v>
       </c>
+      <c r="AA142" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB142" t="s">
         <v>92</v>
       </c>
@@ -36779,7 +37057,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="143" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>217</v>
       </c>
@@ -36852,6 +37130,9 @@
       <c r="AA143" t="s">
         <v>156</v>
       </c>
+      <c r="AB143" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC143" t="s">
         <v>92</v>
       </c>
@@ -36952,7 +37233,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="144" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>287</v>
       </c>
@@ -37025,6 +37306,9 @@
       <c r="AA144" t="s">
         <v>129</v>
       </c>
+      <c r="AB144" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC144" t="s">
         <v>91</v>
       </c>
@@ -37125,7 +37409,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="145" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>146</v>
       </c>
@@ -37198,6 +37482,12 @@
       <c r="Z145" t="s">
         <v>92</v>
       </c>
+      <c r="AA145" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB145" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC145" t="s">
         <v>129</v>
       </c>
@@ -37298,7 +37588,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="146" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>83</v>
       </c>
@@ -37474,7 +37764,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="147" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>268</v>
       </c>
@@ -37544,6 +37834,12 @@
       <c r="Z147" t="s">
         <v>91</v>
       </c>
+      <c r="AA147" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB147" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC147" t="s">
         <v>92</v>
       </c>
@@ -37644,7 +37940,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="148" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>261</v>
       </c>
@@ -37720,6 +38016,12 @@
       <c r="Z148" t="s">
         <v>390</v>
       </c>
+      <c r="AA148" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB148" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC148" t="s">
         <v>92</v>
       </c>
@@ -37820,7 +38122,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="149" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>185</v>
       </c>
@@ -37996,7 +38298,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>270</v>
       </c>
@@ -38172,7 +38474,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="151" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>189</v>
       </c>
@@ -38351,7 +38653,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="152" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>267</v>
       </c>
@@ -38527,7 +38829,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="153" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>229</v>
       </c>
@@ -38597,6 +38899,9 @@
       <c r="Z153" t="s">
         <v>156</v>
       </c>
+      <c r="AA153" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB153" t="s">
         <v>92</v>
       </c>
@@ -38694,7 +38999,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="154" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>163</v>
       </c>
@@ -38870,7 +39175,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="155" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>18</v>
       </c>
@@ -39046,7 +39351,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="156" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>161</v>
       </c>
@@ -39113,6 +39418,12 @@
       <c r="Z156" t="s">
         <v>371</v>
       </c>
+      <c r="AA156" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB156" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC156" t="s">
         <v>371</v>
       </c>
@@ -39213,7 +39524,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="157" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>258</v>
       </c>
@@ -39389,7 +39700,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="158" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>33</v>
       </c>
@@ -39565,7 +39876,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="159" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>181</v>
       </c>
@@ -39741,7 +40052,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="160" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>50</v>
       </c>
@@ -39917,7 +40228,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="161" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>277</v>
       </c>
@@ -40096,7 +40407,7 @@
         <v>2363</v>
       </c>
     </row>
-    <row r="162" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>129</v>
       </c>
@@ -40169,6 +40480,9 @@
       <c r="AA162" t="s">
         <v>92</v>
       </c>
+      <c r="AB162" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC162" t="s">
         <v>129</v>
       </c>
@@ -40269,7 +40583,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="163" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>96</v>
       </c>
@@ -40439,7 +40753,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="164" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>273</v>
       </c>
@@ -40512,6 +40826,9 @@
       <c r="AA164" t="s">
         <v>91</v>
       </c>
+      <c r="AB164" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC164" t="s">
         <v>156</v>
       </c>
@@ -40612,7 +40929,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>207</v>
       </c>
@@ -40682,6 +40999,12 @@
       <c r="Z165" t="s">
         <v>91</v>
       </c>
+      <c r="AA165" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB165" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC165" t="s">
         <v>91</v>
       </c>
@@ -40782,7 +41105,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>7</v>
       </c>
@@ -40852,6 +41175,12 @@
       <c r="Z166" t="s">
         <v>92</v>
       </c>
+      <c r="AA166" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB166" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC166" t="s">
         <v>92</v>
       </c>
@@ -40952,7 +41281,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="167" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>210</v>
       </c>
@@ -41128,7 +41457,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="168" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>220</v>
       </c>
@@ -41198,6 +41527,9 @@
       <c r="Z168" t="s">
         <v>92</v>
       </c>
+      <c r="AA168" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB168" t="s">
         <v>92</v>
       </c>
@@ -41301,7 +41633,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="169" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>201</v>
       </c>
@@ -41477,7 +41809,7 @@
         <v>2463</v>
       </c>
     </row>
-    <row r="170" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>54</v>
       </c>
@@ -41650,7 +41982,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="171" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>134</v>
       </c>
@@ -41826,7 +42158,7 @@
         <v>2490</v>
       </c>
     </row>
-    <row r="172" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>173</v>
       </c>
@@ -42002,7 +42334,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="173" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>168</v>
       </c>
@@ -42178,7 +42510,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="174" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>195</v>
       </c>
@@ -42251,9 +42583,15 @@
       <c r="AA174" t="s">
         <v>92</v>
       </c>
+      <c r="AB174" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC174" t="s">
         <v>92</v>
       </c>
+      <c r="AD174" t="s">
+        <v>3908</v>
+      </c>
       <c r="AE174" t="s">
         <v>99</v>
       </c>
@@ -42348,7 +42686,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="175" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>72</v>
       </c>
@@ -42527,7 +42865,7 @@
         <v>2543</v>
       </c>
     </row>
-    <row r="176" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>143</v>
       </c>
@@ -42703,7 +43041,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="177" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>36</v>
       </c>
@@ -42773,6 +43111,12 @@
       <c r="Z177" t="s">
         <v>371</v>
       </c>
+      <c r="AA177" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB177" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC177" t="s">
         <v>129</v>
       </c>
@@ -42876,7 +43220,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="178" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>151</v>
       </c>
@@ -43052,7 +43396,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="179" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>200</v>
       </c>
@@ -43125,6 +43469,9 @@
       <c r="AA179" t="s">
         <v>129</v>
       </c>
+      <c r="AB179" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC179" t="s">
         <v>92</v>
       </c>
@@ -43225,7 +43572,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="180" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>29</v>
       </c>
@@ -43295,9 +43642,18 @@
       <c r="Z180" t="s">
         <v>92</v>
       </c>
+      <c r="AA180" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB180" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC180" t="s">
         <v>92</v>
       </c>
+      <c r="AD180" t="s">
+        <v>3908</v>
+      </c>
       <c r="AE180" t="s">
         <v>99</v>
       </c>
@@ -43392,7 +43748,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="181" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>170</v>
       </c>
@@ -43568,7 +43924,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="182" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>214</v>
       </c>
@@ -43638,6 +43994,12 @@
       <c r="Z182" t="s">
         <v>92</v>
       </c>
+      <c r="AA182" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB182" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC182" t="s">
         <v>91</v>
       </c>
@@ -43738,7 +44100,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="183" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>57</v>
       </c>
@@ -43914,7 +44276,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="184" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>66</v>
       </c>
@@ -44090,7 +44452,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="185" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>179</v>
       </c>
@@ -44266,7 +44628,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="186" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>142</v>
       </c>
@@ -44336,6 +44698,12 @@
       <c r="Z186" t="s">
         <v>92</v>
       </c>
+      <c r="AA186" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB186" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC186" t="s">
         <v>92</v>
       </c>
@@ -44436,7 +44804,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="187" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>171</v>
       </c>
@@ -44506,6 +44874,12 @@
       <c r="Z187" t="s">
         <v>91</v>
       </c>
+      <c r="AA187" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB187" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC187" t="s">
         <v>91</v>
       </c>
@@ -44606,7 +44980,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="188" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>153</v>
       </c>
@@ -44679,6 +45053,9 @@
       <c r="AA188" t="s">
         <v>129</v>
       </c>
+      <c r="AB188" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC188" t="s">
         <v>92</v>
       </c>
@@ -44779,7 +45156,7 @@
         <v>2704</v>
       </c>
     </row>
-    <row r="189" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>183</v>
       </c>
@@ -44852,6 +45229,9 @@
       <c r="AA189" t="s">
         <v>91</v>
       </c>
+      <c r="AB189" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC189" t="s">
         <v>156</v>
       </c>
@@ -44952,7 +45332,7 @@
         <v>2716</v>
       </c>
     </row>
-    <row r="190" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>112</v>
       </c>
@@ -45128,7 +45508,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="191" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>61</v>
       </c>
@@ -45186,6 +45566,12 @@
       <c r="Z191" t="s">
         <v>129</v>
       </c>
+      <c r="AA191" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB191" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC191" t="s">
         <v>129</v>
       </c>
@@ -45286,7 +45672,7 @@
         <v>2735</v>
       </c>
     </row>
-    <row r="192" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>13</v>
       </c>
@@ -45359,6 +45745,9 @@
       <c r="AA192" t="s">
         <v>129</v>
       </c>
+      <c r="AB192" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC192" t="s">
         <v>156</v>
       </c>
@@ -45459,7 +45848,7 @@
         <v>2751</v>
       </c>
     </row>
-    <row r="193" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>276</v>
       </c>
@@ -45635,7 +46024,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="194" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>197</v>
       </c>
@@ -45708,6 +46097,9 @@
       <c r="AA194" t="s">
         <v>91</v>
       </c>
+      <c r="AB194" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC194" t="s">
         <v>371</v>
       </c>
@@ -45808,7 +46200,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="195" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>216</v>
       </c>
@@ -45984,7 +46376,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="196" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>111</v>
       </c>
@@ -46160,7 +46552,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="197" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>162</v>
       </c>
@@ -46230,6 +46622,12 @@
       <c r="Z197" t="s">
         <v>390</v>
       </c>
+      <c r="AA197" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB197" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC197" t="s">
         <v>156</v>
       </c>
@@ -46330,7 +46728,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="198" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>91</v>
       </c>
@@ -46506,7 +46904,7 @@
         <v>2827</v>
       </c>
     </row>
-    <row r="199" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>285</v>
       </c>
@@ -46576,6 +46974,12 @@
       <c r="Z199" t="s">
         <v>129</v>
       </c>
+      <c r="AA199" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB199" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC199" t="s">
         <v>156</v>
       </c>
@@ -46676,7 +47080,7 @@
         <v>2841</v>
       </c>
     </row>
-    <row r="200" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>166</v>
       </c>
@@ -46852,7 +47256,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="201" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>272</v>
       </c>
@@ -46925,6 +47329,9 @@
       <c r="AA201" t="s">
         <v>129</v>
       </c>
+      <c r="AB201" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC201" t="s">
         <v>91</v>
       </c>
@@ -47025,7 +47432,7 @@
         <v>2866</v>
       </c>
     </row>
-    <row r="202" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>239</v>
       </c>
@@ -47095,6 +47502,9 @@
       <c r="Z202" t="s">
         <v>371</v>
       </c>
+      <c r="AA202" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB202" t="s">
         <v>371</v>
       </c>
@@ -47198,7 +47608,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="203" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>251</v>
       </c>
@@ -47377,7 +47787,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="204" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>222</v>
       </c>
@@ -47553,7 +47963,7 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="205" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>191</v>
       </c>
@@ -47623,6 +48033,12 @@
       <c r="Z205" t="s">
         <v>92</v>
       </c>
+      <c r="AA205" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB205" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC205" t="s">
         <v>91</v>
       </c>
@@ -47723,7 +48139,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="206" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>117</v>
       </c>
@@ -47796,6 +48212,9 @@
       <c r="AA206" t="s">
         <v>92</v>
       </c>
+      <c r="AB206" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC206" t="s">
         <v>92</v>
       </c>
@@ -47896,7 +48315,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="207" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>152</v>
       </c>
@@ -48063,7 +48482,7 @@
         <v>2940</v>
       </c>
     </row>
-    <row r="208" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>31</v>
       </c>
@@ -48239,7 +48658,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>60</v>
       </c>
@@ -48315,6 +48734,9 @@
       <c r="AB209" t="s">
         <v>92</v>
       </c>
+      <c r="AC209" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD209" t="s">
         <v>129</v>
       </c>
@@ -48412,7 +48834,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="210" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>77</v>
       </c>
@@ -48558,7 +48980,7 @@
         <v>2973</v>
       </c>
     </row>
-    <row r="211" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>279</v>
       </c>
@@ -48631,6 +49053,9 @@
       <c r="AA211" t="s">
         <v>92</v>
       </c>
+      <c r="AB211" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC211" t="s">
         <v>156</v>
       </c>
@@ -48719,7 +49144,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="212" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>145</v>
       </c>
@@ -48886,7 +49311,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="213" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>241</v>
       </c>
@@ -49053,7 +49478,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="214" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>192</v>
       </c>
@@ -49129,6 +49554,9 @@
       <c r="AB214" t="s">
         <v>92</v>
       </c>
+      <c r="AC214" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD214" t="s">
         <v>129</v>
       </c>
@@ -49229,7 +49657,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="215" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>85</v>
       </c>
@@ -49393,7 +49821,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="216" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>274</v>
       </c>
@@ -49466,6 +49894,9 @@
       <c r="AA216" t="s">
         <v>91</v>
       </c>
+      <c r="AB216" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC216" t="s">
         <v>91</v>
       </c>
@@ -49554,7 +49985,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="217" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>264</v>
       </c>
@@ -49733,7 +50164,7 @@
         <v>3048</v>
       </c>
     </row>
-    <row r="218" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>188</v>
       </c>
@@ -49803,6 +50234,9 @@
       <c r="Z218" t="s">
         <v>390</v>
       </c>
+      <c r="AA218" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB218" t="s">
         <v>390</v>
       </c>
@@ -49894,7 +50328,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="219" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>32</v>
       </c>
@@ -49967,6 +50401,9 @@
       <c r="AA219" t="s">
         <v>129</v>
       </c>
+      <c r="AB219" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC219" t="s">
         <v>91</v>
       </c>
@@ -50067,7 +50504,7 @@
         <v>3074</v>
       </c>
     </row>
-    <row r="220" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>175</v>
       </c>
@@ -50213,7 +50650,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="221" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>154</v>
       </c>
@@ -50392,7 +50829,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="222" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>114</v>
       </c>
@@ -50465,6 +50902,9 @@
       <c r="AA222" t="s">
         <v>129</v>
       </c>
+      <c r="AB222" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC222" t="s">
         <v>156</v>
       </c>
@@ -50568,7 +51008,7 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="223" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>205</v>
       </c>
@@ -50744,7 +51184,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="224" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>198</v>
       </c>
@@ -50911,7 +51351,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="225" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>187</v>
       </c>
@@ -50984,6 +51424,9 @@
       <c r="AA225" t="s">
         <v>91</v>
       </c>
+      <c r="AB225" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC225" t="s">
         <v>390</v>
       </c>
@@ -51084,7 +51527,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="226" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>137</v>
       </c>
@@ -51263,7 +51706,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="227" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>147</v>
       </c>
@@ -51442,7 +51885,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="228" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>233</v>
       </c>
@@ -51515,6 +51958,9 @@
       <c r="AA228" t="s">
         <v>92</v>
       </c>
+      <c r="AB228" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC228" t="s">
         <v>91</v>
       </c>
@@ -51618,7 +52064,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="229" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>271</v>
       </c>
@@ -51797,7 +52243,7 @@
         <v>2735</v>
       </c>
     </row>
-    <row r="230" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>3</v>
       </c>
@@ -51973,7 +52419,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="231" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>115</v>
       </c>
@@ -52149,7 +52595,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="232" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>89</v>
       </c>
@@ -52225,6 +52671,9 @@
       <c r="AB232" t="s">
         <v>92</v>
       </c>
+      <c r="AC232" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD232" t="s">
         <v>129</v>
       </c>
@@ -52310,7 +52759,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="233" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>79</v>
       </c>
@@ -52380,6 +52829,9 @@
       <c r="Z233" t="s">
         <v>91</v>
       </c>
+      <c r="AA233" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB233" t="s">
         <v>92</v>
       </c>
@@ -52474,7 +52926,7 @@
         <v>3245</v>
       </c>
     </row>
-    <row r="234" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>2</v>
       </c>
@@ -52617,7 +53069,7 @@
         <v>3253</v>
       </c>
     </row>
-    <row r="235" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>121</v>
       </c>
@@ -52784,7 +53236,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="236" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>84</v>
       </c>
@@ -52951,7 +53403,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="237" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>155</v>
       </c>
@@ -53115,7 +53567,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="238" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>12</v>
       </c>
@@ -53261,7 +53713,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="239" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>228</v>
       </c>
@@ -53419,7 +53871,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="240" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>126</v>
       </c>
@@ -53598,7 +54050,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="241" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>218</v>
       </c>
@@ -53777,7 +54229,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="242" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>47</v>
       </c>
@@ -53850,6 +54302,9 @@
       <c r="AA242" t="s">
         <v>92</v>
       </c>
+      <c r="AB242" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC242" t="s">
         <v>92</v>
       </c>
@@ -53953,7 +54408,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="243" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>55</v>
       </c>
@@ -54132,7 +54587,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="244" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>246</v>
       </c>
@@ -54205,6 +54660,9 @@
       <c r="AA244" t="s">
         <v>92</v>
       </c>
+      <c r="AB244" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC244" t="s">
         <v>91</v>
       </c>
@@ -54293,7 +54751,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="245" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>25</v>
       </c>
@@ -54369,6 +54827,9 @@
       <c r="AB245" t="s">
         <v>129</v>
       </c>
+      <c r="AC245" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD245" t="s">
         <v>92</v>
       </c>
@@ -54457,7 +54918,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="246" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>9</v>
       </c>
@@ -54530,6 +54991,9 @@
       <c r="AA246" t="s">
         <v>92</v>
       </c>
+      <c r="AB246" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC246" t="s">
         <v>92</v>
       </c>
@@ -54618,7 +55082,7 @@
         <v>3074</v>
       </c>
     </row>
-    <row r="247" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>106</v>
       </c>
@@ -54797,7 +55261,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="248" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>236</v>
       </c>
@@ -54870,6 +55334,9 @@
       <c r="AA248" t="s">
         <v>92</v>
       </c>
+      <c r="AB248" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC248" t="s">
         <v>371</v>
       </c>
@@ -54961,7 +55428,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="249" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>280</v>
       </c>
@@ -55034,9 +55501,15 @@
       <c r="AA249" t="s">
         <v>129</v>
       </c>
+      <c r="AB249" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC249" t="s">
         <v>92</v>
       </c>
+      <c r="AD249" t="s">
+        <v>3908</v>
+      </c>
       <c r="AH249" t="s">
         <v>99</v>
       </c>
@@ -55134,7 +55607,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="250" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>27</v>
       </c>
@@ -55307,7 +55780,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="251" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>123</v>
       </c>
@@ -55377,6 +55850,12 @@
       <c r="Z251" t="s">
         <v>371</v>
       </c>
+      <c r="AA251" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB251" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC251" t="s">
         <v>156</v>
       </c>
@@ -55480,7 +55959,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="252" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>178</v>
       </c>
@@ -55550,6 +56029,12 @@
       <c r="Z252" t="s">
         <v>92</v>
       </c>
+      <c r="AA252" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB252" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC252" t="s">
         <v>92</v>
       </c>
@@ -55653,7 +56138,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="253" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>196</v>
       </c>
@@ -55832,7 +56317,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="254" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>243</v>
       </c>
@@ -55999,7 +56484,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="255" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>44</v>
       </c>
@@ -56178,7 +56663,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="256" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>221</v>
       </c>
@@ -56357,7 +56842,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="257" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>76</v>
       </c>
@@ -56430,6 +56915,9 @@
       <c r="AA257" t="s">
         <v>92</v>
       </c>
+      <c r="AB257" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC257" t="s">
         <v>156</v>
       </c>
@@ -56533,7 +57021,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="258" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>34</v>
       </c>
@@ -56700,7 +57188,7 @@
         <v>3531</v>
       </c>
     </row>
-    <row r="259" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>35</v>
       </c>
@@ -56879,7 +57367,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="260" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>64</v>
       </c>
@@ -57061,7 +57549,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="261" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>10</v>
       </c>
@@ -57131,6 +57619,9 @@
       <c r="Z261" t="s">
         <v>156</v>
       </c>
+      <c r="AA261" t="s">
+        <v>3908</v>
+      </c>
       <c r="AB261" t="s">
         <v>156</v>
       </c>
@@ -57237,7 +57728,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="262" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>1</v>
       </c>
@@ -57416,7 +57907,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="263" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>224</v>
       </c>
@@ -57595,7 +58086,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="264" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>266</v>
       </c>
@@ -57774,7 +58265,7 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="265" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>67</v>
       </c>
@@ -57953,7 +58444,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="266" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>41</v>
       </c>
@@ -58023,6 +58514,12 @@
       <c r="Z266" t="s">
         <v>92</v>
       </c>
+      <c r="AA266" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB266" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC266" t="s">
         <v>91</v>
       </c>
@@ -58117,7 +58614,7 @@
         <v>3627</v>
       </c>
     </row>
-    <row r="267" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>5</v>
       </c>
@@ -58296,7 +58793,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="268" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>120</v>
       </c>
@@ -58475,7 +58972,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="269" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>15</v>
       </c>
@@ -58551,6 +59048,9 @@
       <c r="AB269" t="s">
         <v>92</v>
       </c>
+      <c r="AC269" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD269" t="s">
         <v>92</v>
       </c>
@@ -58651,7 +59151,7 @@
         <v>3664</v>
       </c>
     </row>
-    <row r="270" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>244</v>
       </c>
@@ -58830,7 +59330,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="271" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>290</v>
       </c>
@@ -58903,6 +59403,9 @@
       <c r="AA271" t="s">
         <v>129</v>
       </c>
+      <c r="AB271" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC271" t="s">
         <v>91</v>
       </c>
@@ -59006,7 +59509,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="272" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>104</v>
       </c>
@@ -59137,7 +59640,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="273" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>164</v>
       </c>
@@ -59301,7 +59804,7 @@
         <v>3689</v>
       </c>
     </row>
-    <row r="274" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>122</v>
       </c>
@@ -59447,7 +59950,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="275" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>227</v>
       </c>
@@ -59623,7 +60126,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="276" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>37</v>
       </c>
@@ -59802,7 +60305,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="277" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>6</v>
       </c>
@@ -59872,6 +60375,9 @@
       <c r="AA277" t="s">
         <v>129</v>
       </c>
+      <c r="AB277" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC277" t="s">
         <v>92</v>
       </c>
@@ -59975,7 +60481,7 @@
         <v>3737</v>
       </c>
     </row>
-    <row r="278" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>113</v>
       </c>
@@ -60139,7 +60645,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="279" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>278</v>
       </c>
@@ -60306,7 +60812,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="280" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>141</v>
       </c>
@@ -60482,7 +60988,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="281" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>68</v>
       </c>
@@ -60661,7 +61167,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="282" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>263</v>
       </c>
@@ -60840,7 +61346,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="283" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>186</v>
       </c>
@@ -60913,6 +61419,9 @@
       <c r="AA283" t="s">
         <v>92</v>
       </c>
+      <c r="AB283" t="s">
+        <v>3908</v>
+      </c>
       <c r="AC283" t="s">
         <v>156</v>
       </c>
@@ -61004,7 +61513,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="284" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>26</v>
       </c>
@@ -61180,7 +61689,7 @@
         <v>3820</v>
       </c>
     </row>
-    <row r="285" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>156</v>
       </c>
@@ -61356,7 +61865,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>211</v>
       </c>
@@ -61529,7 +62038,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="287" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>177</v>
       </c>
@@ -61599,6 +62108,15 @@
       <c r="Z287" t="s">
         <v>92</v>
       </c>
+      <c r="AA287" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AB287" t="s">
+        <v>3908</v>
+      </c>
+      <c r="AC287" t="s">
+        <v>3908</v>
+      </c>
       <c r="AD287" t="s">
         <v>91</v>
       </c>
@@ -61696,7 +62214,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="288" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>138</v>
       </c>
@@ -61875,7 +62393,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="289" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>208</v>
       </c>
@@ -62054,7 +62572,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="290" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>97</v>
       </c>
@@ -62221,7 +62739,7 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="291" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>107</v>
       </c>

</xml_diff>